<commit_message>
terminacion analisis simulacion base
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/analisis/Resultados_analisis/Multi_d/2_tabla_d_vs_modelo.xlsx
+++ b/codigo_final_organizado/analisis/Resultados_analisis/Multi_d/2_tabla_d_vs_modelo.xlsx
@@ -438,25 +438,25 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>92.34260158568215</v>
+        <v>90.33701601336995</v>
       </c>
       <c r="C2">
-        <v>99.28376079120463</v>
+        <v>97.99789108864614</v>
       </c>
       <c r="D2">
-        <v>99.04156088578041</v>
+        <v>99.25719803621033</v>
       </c>
       <c r="E2">
-        <v>98.54126426417911</v>
+        <v>98.72966839909351</v>
       </c>
       <c r="F2">
-        <v>98.04299270369691</v>
+        <v>98.23074575766434</v>
       </c>
       <c r="G2">
-        <v>97.09164267137373</v>
+        <v>97.28828811886578</v>
       </c>
       <c r="H2">
-        <v>95.68110608224315</v>
+        <v>95.86270046195699</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -464,25 +464,25 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>77.33186396226384</v>
+        <v>76.89876022041162</v>
       </c>
       <c r="C3">
-        <v>99.11804553087575</v>
+        <v>94.07007365722883</v>
       </c>
       <c r="D3">
-        <v>98.81032195380843</v>
+        <v>99.00016420823033</v>
       </c>
       <c r="E3">
-        <v>98.70924544345435</v>
+        <v>98.71570471705476</v>
       </c>
       <c r="F3">
-        <v>98.34739658906591</v>
+        <v>98.45910039451762</v>
       </c>
       <c r="G3">
-        <v>97.56147285089145</v>
+        <v>97.55691708871703</v>
       </c>
       <c r="H3">
-        <v>96.24417315761396</v>
+        <v>96.12898886077714</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -490,25 +490,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>93.53615765227777</v>
+        <v>91.92264418048704</v>
       </c>
       <c r="C4">
-        <v>99.27011437231891</v>
+        <v>98.13284670726674</v>
       </c>
       <c r="D4">
-        <v>99.01671680091304</v>
+        <v>99.23778052608313</v>
       </c>
       <c r="E4">
-        <v>98.51726285604573</v>
+        <v>98.71004261302667</v>
       </c>
       <c r="F4">
-        <v>98.02595957477519</v>
+        <v>98.21268306562727</v>
       </c>
       <c r="G4">
-        <v>97.07686261185563</v>
+        <v>97.2763229845675</v>
       </c>
       <c r="H4">
-        <v>95.6704939297569</v>
+        <v>95.85348005711388</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -516,25 +516,25 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>81.07446806829267</v>
+        <v>78.53890916540075</v>
       </c>
       <c r="C5">
-        <v>99.64711021651428</v>
+        <v>97.06733670160607</v>
       </c>
       <c r="D5">
-        <v>99.24240636568112</v>
+        <v>99.41478311448603</v>
       </c>
       <c r="E5">
-        <v>98.65045205946872</v>
+        <v>98.8559289049183</v>
       </c>
       <c r="F5">
-        <v>98.12567829120691</v>
+        <v>98.30016816553849</v>
       </c>
       <c r="G5">
-        <v>97.15834954982721</v>
+        <v>97.32977735399146</v>
       </c>
       <c r="H5">
-        <v>95.71241775091036</v>
+        <v>95.88960392010006</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -542,25 +542,25 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>86.37892082562416</v>
+        <v>85.39860290829367</v>
       </c>
       <c r="C6">
-        <v>98.51278501504977</v>
+        <v>95.47603018624659</v>
       </c>
       <c r="D6">
-        <v>98.72606324878005</v>
+        <v>99.03557576777675</v>
       </c>
       <c r="E6">
-        <v>98.54736162461283</v>
+        <v>98.57199874879504</v>
       </c>
       <c r="F6">
-        <v>98.18482880135902</v>
+        <v>98.31066284644379</v>
       </c>
       <c r="G6">
-        <v>97.57074921349387</v>
+        <v>97.56666974420268</v>
       </c>
       <c r="H6">
-        <v>96.32787001014842</v>
+        <v>96.2247806100732</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -568,25 +568,25 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>49.94545140146874</v>
+        <v>41.39579404654932</v>
       </c>
       <c r="C7">
-        <v>97.81078727517621</v>
+        <v>50.28889861122961</v>
       </c>
       <c r="D7">
-        <v>99.98248559575444</v>
+        <v>98.82604622396775</v>
       </c>
       <c r="E7">
-        <v>99.98815899947861</v>
+        <v>98.92103190527189</v>
       </c>
       <c r="F7">
-        <v>99.96409114640807</v>
+        <v>98.49091268988114</v>
       </c>
       <c r="G7">
-        <v>99.7837026351409</v>
+        <v>97.59349024792978</v>
       </c>
       <c r="H7">
-        <v>99.49330382332168</v>
+        <v>96.19316105527326</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -594,25 +594,25 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>76.80115576213386</v>
+        <v>79.57218880010741</v>
       </c>
       <c r="C8">
-        <v>98.00746476305667</v>
+        <v>86.35384427366763</v>
       </c>
       <c r="D8">
-        <v>99.31993326451837</v>
+        <v>99.32680854529019</v>
       </c>
       <c r="E8">
-        <v>98.95527873386742</v>
+        <v>98.92216067459138</v>
       </c>
       <c r="F8">
-        <v>98.54175641638889</v>
+        <v>98.47245700686243</v>
       </c>
       <c r="G8">
-        <v>97.72032879553917</v>
+        <v>97.56316972844064</v>
       </c>
       <c r="H8">
-        <v>96.49903745548191</v>
+        <v>96.13267281987892</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -620,25 +620,25 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>76.047680279723</v>
+        <v>74.61769130626827</v>
       </c>
       <c r="C9">
-        <v>99.32013576668072</v>
+        <v>95.16083180530659</v>
       </c>
       <c r="D9">
-        <v>99.23774520726614</v>
+        <v>99.37025810399646</v>
       </c>
       <c r="E9">
-        <v>98.77044981660654</v>
+        <v>98.88526414555285</v>
       </c>
       <c r="F9">
-        <v>98.28273742234344</v>
+        <v>98.40341225926801</v>
       </c>
       <c r="G9">
-        <v>97.34421106260909</v>
+        <v>97.4590900614585</v>
       </c>
       <c r="H9">
-        <v>95.94367462309978</v>
+        <v>96.02337987804562</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -646,25 +646,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.3369539794865306</v>
+        <v>0.1688198682658943</v>
       </c>
       <c r="C10">
-        <v>0.04277642293854379</v>
+        <v>0.04790827893590049</v>
       </c>
       <c r="D10">
-        <v>0.02267769269317164</v>
+        <v>-0.001756253530937295</v>
       </c>
       <c r="E10">
-        <v>0.01658380981634526</v>
+        <v>0.01675237852423847</v>
       </c>
       <c r="F10">
-        <v>78.2513769210066</v>
+        <v>18.26692517429614</v>
       </c>
       <c r="G10">
-        <v>97.52354688663017</v>
+        <v>98.11386914362433</v>
       </c>
       <c r="H10">
-        <v>96.23861186200017</v>
+        <v>95.52771486509967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>